<commit_message>
Removed Aspmes, added pyrmes
Removed Aspmes from target compound list and MDV files.  Added Pyrmes (alanine data).  Model runs, but fluxes aren't meaningful yet.
</commit_message>
<xml_diff>
--- a/data_elimosum/Aug2022Bicarb_AA_MFA_1.xlsx
+++ b/data_elimosum/Aug2022Bicarb_AA_MFA_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Xoots/__Experiment_Data/C1MFA/data_Elimosum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Xoots/__Experiment_Data/Carbon-Flux-Team/data_elimosum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{289592AF-3997-DE4E-8019-B6175AE32E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D51A286-E985-754F-AF66-CE4A9FF308E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="460" windowWidth="27240" windowHeight="15320" activeTab="1"/>
+    <workbookView xWindow="660" yWindow="460" windowWidth="27240" windowHeight="15320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aug2022Bicarb_AA_MFA_1" sheetId="1" r:id="rId1"/>
@@ -300,7 +300,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1134,7 +1134,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD275"/>
   <sheetViews>
     <sheetView topLeftCell="A204" workbookViewId="0">
@@ -8867,11 +8867,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>